<commit_message>
Paper is finished.  Final submission
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/9438/School/Spring2020/CSCI5922/final_project/final_timothy_mason_csci5922_s20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8C657C-304C-2F48-802D-E6A29455D358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B99687-F51D-E24F-944C-AE45E747C714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="3" xr2:uid="{F58C6C7F-5855-FD4B-B1F8-9C76888EB29A}"/>
   </bookViews>
@@ -17,8 +17,9 @@
     <sheet name="Hyperparm Train Results" sheetId="6" r:id="rId2"/>
     <sheet name="Rep Data" sheetId="5" r:id="rId3"/>
     <sheet name="Repeatability" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,61 +37,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
-    <t>80k parms, feat. len. 252</t>
+    <t>segments</t>
   </si>
   <si>
-    <t>2.5M parms, feat. len. 252</t>
+    <t>Remaining Songs</t>
   </si>
   <si>
-    <t>2.5M parms, feat. len. 512</t>
+    <t>Layer</t>
   </si>
   <si>
-    <t>2.5M parms, feat. len. 1024</t>
+    <t>Smaller Model
+(N)</t>
   </si>
   <si>
-    <t>80k parms, feat. len. 512</t>
+    <t>Large Model 
+(N)</t>
   </si>
   <si>
-    <t>80k parms, feat. len. 1024</t>
+    <t>conv2d</t>
   </si>
   <si>
-    <t>2.5M, 1024, 100 Epoch, #1</t>
+    <t>rnn</t>
   </si>
   <si>
-    <t>2.5M, 1024, 100 Epoch, #2</t>
+    <t>Smaller Model parms, segments=252</t>
   </si>
   <si>
-    <t>2.5M, 1024, 100 Epoch, #3</t>
+    <t>Smaller Model parms, segments=512</t>
   </si>
   <si>
-    <t>2.5M, 1024, 100 Epoch, #4</t>
+    <t>Smaller Model parms, segments=1024</t>
   </si>
   <si>
-    <t>2.5M, 1024, 100 Epoch, #5</t>
+    <t>Large Model, segments=252</t>
   </si>
   <si>
-    <t>2.5M, 252, 100 Epoch, #1</t>
+    <t>Large Model, segments=512</t>
   </si>
   <si>
-    <t>2.5M, 252, 100 Epoch, #2</t>
+    <t>Large Model, segments=1024</t>
   </si>
   <si>
-    <t>2.5M, 252, 100 Epoch, #3</t>
+    <t>Large, 1024, 100 Epoch, #1</t>
   </si>
   <si>
-    <t>2.5M, 252, 100 Epoch, #4</t>
+    <t>Large, 1024, 100 Epoch, #2</t>
   </si>
   <si>
-    <t>2.5M, 252, 100 Epoch, #5</t>
+    <t>Large, 1024, 100 Epoch, #3</t>
+  </si>
+  <si>
+    <t>Large, 1024, 100 Epoch, #4</t>
+  </si>
+  <si>
+    <t>Large, 1024, 100 Epoch, #5</t>
+  </si>
+  <si>
+    <t>Large, 252, 100 Epoch, #1</t>
+  </si>
+  <si>
+    <t>Large, 252, 100 Epoch, #2</t>
+  </si>
+  <si>
+    <t>Large, 252, 100 Epoch, #3</t>
+  </si>
+  <si>
+    <t>Large, 252, 100 Epoch, #4</t>
+  </si>
+  <si>
+    <t>Large, 252, 100 Epoch, #5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,16 +130,35 @@
       <name val="HelveticaNeue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="HelveticaNeue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="HelveticaNeue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,17 +166,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -171,7 +251,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80k parms, feat. len. 252</c:v>
+                  <c:v>Smaller Model parms, segments=252</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -375,7 +455,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M parms, feat. len. 252</c:v>
+                  <c:v>Large Model, segments=252</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -579,7 +659,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80k parms, feat. len. 512</c:v>
+                  <c:v>Smaller Model parms, segments=512</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -783,7 +863,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M parms, feat. len. 512</c:v>
+                  <c:v>Large Model, segments=512</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -987,7 +1067,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80k parms, feat. len. 1024</c:v>
+                  <c:v>Smaller Model parms, segments=1024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1191,7 +1271,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M parms, feat. len. 1024</c:v>
+                  <c:v>Large Model, segments=1024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1633,10 +1713,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.74737171968302107"/>
-          <c:y val="0.59046148737904203"/>
-          <c:w val="0.19190559582161179"/>
-          <c:h val="0.20467884567908015"/>
+          <c:x val="0.60523609236519738"/>
+          <c:y val="0.5015152535309888"/>
+          <c:w val="0.25931012011666221"/>
+          <c:h val="0.20670035099380862"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1750,7 +1830,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 1024, 100 Epoch, #1</c:v>
+                  <c:v>Large, 1024, 100 Epoch, #1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2092,7 +2172,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 1024, 100 Epoch, #2</c:v>
+                  <c:v>Large, 1024, 100 Epoch, #2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2434,7 +2514,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 1024, 100 Epoch, #3</c:v>
+                  <c:v>Large, 1024, 100 Epoch, #3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2776,7 +2856,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 1024, 100 Epoch, #4</c:v>
+                  <c:v>Large, 1024, 100 Epoch, #4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3118,7 +3198,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 1024, 100 Epoch, #5</c:v>
+                  <c:v>Large, 1024, 100 Epoch, #5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3460,7 +3540,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 252, 100 Epoch, #1</c:v>
+                  <c:v>Large, 252, 100 Epoch, #1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3802,7 +3882,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 252, 100 Epoch, #2</c:v>
+                  <c:v>Large, 252, 100 Epoch, #2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4146,7 +4226,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 252, 100 Epoch, #3</c:v>
+                  <c:v>Large, 252, 100 Epoch, #3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4490,7 +4570,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 252, 100 Epoch, #4</c:v>
+                  <c:v>Large, 252, 100 Epoch, #4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4834,7 +4914,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5M, 252, 100 Epoch, #5</c:v>
+                  <c:v>Large, 252, 100 Epoch, #5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6671,12 +6751,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7528F41-804E-7E48-9733-826563A237B7}" name="Table1" displayName="Table1" ref="A1:F51" totalsRowShown="0">
   <autoFilter ref="A1:F51" xr:uid="{79D92982-3207-7049-8A9E-007E2456E835}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{827702AC-DB8D-5643-BCDA-8BB05A2BF87E}" name="80k parms, feat. len. 252"/>
-    <tableColumn id="3" xr3:uid="{F45270DC-9EB0-F741-A3FD-CD70B930B5C0}" name="2.5M parms, feat. len. 252"/>
-    <tableColumn id="7" xr3:uid="{C68F05C9-4F45-6741-B191-781D16B5FC04}" name="80k parms, feat. len. 512"/>
-    <tableColumn id="4" xr3:uid="{77683BC3-BF26-224D-8708-03A367D12606}" name="2.5M parms, feat. len. 512"/>
-    <tableColumn id="8" xr3:uid="{C661BF7A-415F-7148-8159-ABF5468081A4}" name="80k parms, feat. len. 1024"/>
-    <tableColumn id="5" xr3:uid="{161FB794-8ACB-1E42-9A1D-2D1530D1DDA0}" name="2.5M parms, feat. len. 1024"/>
+    <tableColumn id="1" xr3:uid="{827702AC-DB8D-5643-BCDA-8BB05A2BF87E}" name="Smaller Model parms, segments=252"/>
+    <tableColumn id="3" xr3:uid="{F45270DC-9EB0-F741-A3FD-CD70B930B5C0}" name="Large Model, segments=252"/>
+    <tableColumn id="7" xr3:uid="{C68F05C9-4F45-6741-B191-781D16B5FC04}" name="Smaller Model parms, segments=512"/>
+    <tableColumn id="4" xr3:uid="{77683BC3-BF26-224D-8708-03A367D12606}" name="Large Model, segments=512"/>
+    <tableColumn id="8" xr3:uid="{C661BF7A-415F-7148-8159-ABF5468081A4}" name="Smaller Model parms, segments=1024"/>
+    <tableColumn id="5" xr3:uid="{161FB794-8ACB-1E42-9A1D-2D1530D1DDA0}" name="Large Model, segments=1024"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6686,18 +6766,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77B58BBF-E3CE-EA4A-B666-21C4B2546EEA}" name="Table13" displayName="Table13" ref="A1:J102" totalsRowShown="0">
   <autoFilter ref="A1:J102" xr:uid="{79D92982-3207-7049-8A9E-007E2456E835}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B3427008-7793-384E-8AB9-5524BC8848C0}" name="2.5M, 1024, 100 Epoch, #1"/>
-    <tableColumn id="3" xr3:uid="{024E4631-B962-DC4A-A43B-884355ECDDBE}" name="2.5M, 1024, 100 Epoch, #2"/>
-    <tableColumn id="7" xr3:uid="{C3A54F55-FD26-404D-B88A-D4237149B25E}" name="2.5M, 1024, 100 Epoch, #3"/>
-    <tableColumn id="4" xr3:uid="{87A99A2E-F145-D74F-9895-9669F29DE6A6}" name="2.5M, 1024, 100 Epoch, #4"/>
-    <tableColumn id="8" xr3:uid="{C3771930-0C4E-B347-B345-71E8F2D848A6}" name="2.5M, 1024, 100 Epoch, #5"/>
-    <tableColumn id="5" xr3:uid="{9702DCD8-ABB6-F244-87C2-83A39C1954BB}" name="2.5M, 252, 100 Epoch, #1"/>
-    <tableColumn id="10" xr3:uid="{B03179F7-3B20-CF4B-99E8-7480CD8F55B3}" name="2.5M, 252, 100 Epoch, #2"/>
-    <tableColumn id="11" xr3:uid="{B8FFB89E-DEE5-C64E-BC67-3D8C55312FB5}" name="2.5M, 252, 100 Epoch, #3"/>
-    <tableColumn id="12" xr3:uid="{AFD3C687-8B84-BA4D-B578-589DF89C086B}" name="2.5M, 252, 100 Epoch, #4"/>
-    <tableColumn id="13" xr3:uid="{B4FB0CF4-5230-714A-9D90-7EAD82E03C84}" name="2.5M, 252, 100 Epoch, #5"/>
+    <tableColumn id="1" xr3:uid="{B3427008-7793-384E-8AB9-5524BC8848C0}" name="Large, 1024, 100 Epoch, #1"/>
+    <tableColumn id="3" xr3:uid="{024E4631-B962-DC4A-A43B-884355ECDDBE}" name="Large, 1024, 100 Epoch, #2"/>
+    <tableColumn id="7" xr3:uid="{C3A54F55-FD26-404D-B88A-D4237149B25E}" name="Large, 1024, 100 Epoch, #3"/>
+    <tableColumn id="4" xr3:uid="{87A99A2E-F145-D74F-9895-9669F29DE6A6}" name="Large, 1024, 100 Epoch, #4"/>
+    <tableColumn id="8" xr3:uid="{C3771930-0C4E-B347-B345-71E8F2D848A6}" name="Large, 1024, 100 Epoch, #5"/>
+    <tableColumn id="5" xr3:uid="{9702DCD8-ABB6-F244-87C2-83A39C1954BB}" name="Large, 252, 100 Epoch, #1"/>
+    <tableColumn id="10" xr3:uid="{B03179F7-3B20-CF4B-99E8-7480CD8F55B3}" name="Large, 252, 100 Epoch, #2"/>
+    <tableColumn id="11" xr3:uid="{B8FFB89E-DEE5-C64E-BC67-3D8C55312FB5}" name="Large, 252, 100 Epoch, #3"/>
+    <tableColumn id="12" xr3:uid="{AFD3C687-8B84-BA4D-B578-589DF89C086B}" name="Large, 252, 100 Epoch, #4"/>
+    <tableColumn id="13" xr3:uid="{B4FB0CF4-5230-714A-9D90-7EAD82E03C84}" name="Large, 252, 100 Epoch, #5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{63BB2497-E72D-8C41-A482-8E6DCABB1763}" name="Table3" displayName="Table3" ref="A1:B4" totalsRowShown="0" dataDxfId="0" dataCellStyle="Comma">
+  <autoFilter ref="A1:B4" xr:uid="{97F5442B-8A37-DC40-84BE-AF10B4B4FBDD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{450FBACE-C6CD-804C-8B68-FE9F2CFA1466}" name="segments" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{D410ED74-CEA3-CE4B-A295-0999F5D9F5B5}" name="Remaining Songs" dataDxfId="1" dataCellStyle="Comma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -7001,7 +7092,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7016,22 +7107,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -8047,8 +8138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9B6F77-E557-6B48-9B37-C4BCEEDFEC01}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J101"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8063,34 +8154,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -11300,4 +11391,132 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E254176-DA85-C94E-B066-8CFB80D1D45D}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="E10:G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B2" s="1">
+        <v>587</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>512</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2049</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>252</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2243</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="34">
+      <c r="E10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>60</v>
+      </c>
+      <c r="G11" s="4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>60</v>
+      </c>
+      <c r="G12" s="4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>60</v>
+      </c>
+      <c r="G13" s="4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>30</v>
+      </c>
+      <c r="G14" s="4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4">
+        <v>30</v>
+      </c>
+      <c r="G15" s="4">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>